<commit_message>
Bugfix to drfit correction
</commit_message>
<xml_diff>
--- a/inst/extdata/split_data.xlsx
+++ b/inst/extdata/split_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CF927A-EAF3-4348-8692-FA63CD9A50F6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100B3D7A-D2C8-4302-BCAC-0A0D92B4EF4B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="612" yWindow="2400" windowWidth="23016" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1778,7 +1778,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1993,9 +1993,6 @@
       <c r="I5">
         <v>51000</v>
       </c>
-      <c r="J5">
-        <v>52000</v>
-      </c>
       <c r="K5">
         <v>53000</v>
       </c>

</xml_diff>